<commit_message>
docs: Updating junheon status
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Documents\GitHub\BOJ_Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D076DCE-52DD-4146-8579-BFB44509D5A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C263FB-A949-44EF-8E0C-289F79998E87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FAC882FD-80ED-4FED-BC86-1169BB2BEEB8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
   <si>
     <t>난이도</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -83,94 +83,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>스택</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>날짜</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>단어 뒤집기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>괄호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스택 수열</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>에디터</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>큐</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>조세퍼스 문제</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>덱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>단어 뒤집기 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>쇠막대기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오큰수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>오등큰수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>후위 표기식 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>후위 표기식</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>알파벳 개수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>알파벳 찾기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>문자열 분석</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>단어 길이 재기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ROT13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네 수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>접미사 배열</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>문자열</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -179,19 +95,115 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>나머지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최대공약수와 최소공배수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>최소공배수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>소수 찾기</t>
+    <t>10828 스택</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9093 단어 뒤집기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9012 괄호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1874 스택 수열</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1406 에디터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10845 큐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1158 조세퍼스 문제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10866 덱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17413 단어 뒤집기 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10799 쇠막대기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17298 오큰수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17299 오등큰수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1935 후위 표기식 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1918 후위 표기식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10808 알파벳 개수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10809 알파벳 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10820 문자열 분석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2743 단어 길이 재기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11655 ROT13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10824 네 수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11656 접미사 배열</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10430 나머지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2609 최대공약수와 최소공배수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1934 최소공배수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1978 소수 찾기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1929 소수 구하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6588 골드바흐의 추측</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10872 팩토리얼</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -616,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A455562-4D3A-4B25-96ED-E97C9A43915F}">
   <dimension ref="A1:J351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:D26"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -639,7 +651,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="2"/>
@@ -656,7 +668,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D2" s="5">
         <v>44191</v>
@@ -670,7 +682,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D3" s="5">
         <v>44191</v>
@@ -684,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="5">
         <v>44191</v>
@@ -698,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="5">
         <v>44191</v>
@@ -712,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="5">
         <v>44191</v>
@@ -726,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" s="5">
         <v>44191</v>
@@ -740,7 +752,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5">
         <v>44191</v>
@@ -754,7 +766,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D9" s="5">
         <v>44191</v>
@@ -768,7 +780,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D10" s="5">
         <v>44191</v>
@@ -782,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5">
         <v>44191</v>
@@ -796,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D12" s="5">
         <v>44191</v>
@@ -810,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5">
         <v>44191</v>
@@ -824,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D14" s="5">
         <v>44191</v>
@@ -838,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D15" s="5">
         <v>44191</v>
@@ -846,13 +858,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D16" s="5">
         <v>44191</v>
@@ -860,13 +872,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D17" s="5">
         <v>44191</v>
@@ -874,13 +886,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B18" s="4">
         <v>1</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D18" s="5">
         <v>44192</v>
@@ -888,13 +900,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D19" s="5">
         <v>44192</v>
@@ -902,13 +914,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B20" s="4">
         <v>1</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D20" s="5">
         <v>44192</v>
@@ -916,13 +928,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D21" s="5">
         <v>44192</v>
@@ -930,13 +942,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B22" s="4">
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D22" s="5">
         <v>44192</v>
@@ -944,7 +956,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
@@ -958,7 +970,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
@@ -972,7 +984,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B25" s="4">
         <v>1</v>
@@ -986,7 +998,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B26" s="4">
         <v>1</v>
@@ -999,22 +1011,46 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
+      <c r="A27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="5">
+        <v>44195</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
+      <c r="A28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="5">
+        <v>44195</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
+      <c r="A29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="5">
+        <v>44195</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="4"/>

</xml_diff>

<commit_message>
docs: Uploading junheon status
</commit_message>
<xml_diff>
--- a/Status.xlsx
+++ b/Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSI\Documents\GitHub\BOJ_Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A668DF-6AB2-4D05-A66A-4558834E3033}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F319FE-270D-4CF2-85B6-B762232BB0A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FAC882FD-80ED-4FED-BC86-1169BB2BEEB8}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="83">
   <si>
     <t>난이도</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -345,6 +345,30 @@
   </si>
   <si>
     <t>RGB거리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10007 * 10 해봤자 100000인데 왜 long long 이지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동물원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오르막 수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스티커</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포도주 시식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정수 삼각형</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -772,8 +796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A455562-4D3A-4B25-96ED-E97C9A43915F}">
   <dimension ref="A1:J347"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="C49" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -783,7 +807,7 @@
     <col min="3" max="4" width="8.6640625" style="3"/>
     <col min="5" max="5" width="45.9140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.9140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="41.4140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1946,25 +1970,103 @@
       <c r="A58" s="3">
         <v>57</v>
       </c>
+      <c r="B58" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58" s="3">
+        <v>2</v>
+      </c>
+      <c r="D58" s="3">
+        <v>1309</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F58" s="4">
+        <v>44209</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="3">
         <v>58</v>
       </c>
+      <c r="B59" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="3">
+        <v>1</v>
+      </c>
+      <c r="D59" s="3">
+        <v>11057</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F59" s="4">
+        <v>44209</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="3">
         <v>59</v>
       </c>
+      <c r="B60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="3">
+        <v>1</v>
+      </c>
+      <c r="D60" s="3">
+        <v>9465</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F60" s="4">
+        <v>44209</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="3">
         <v>60</v>
       </c>
+      <c r="B61" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="3">
+        <v>2</v>
+      </c>
+      <c r="D61" s="3">
+        <v>2156</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F61" s="4">
+        <v>44209</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="3">
         <v>61</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="3">
+        <v>1</v>
+      </c>
+      <c r="D62" s="3">
+        <v>1932</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F62" s="4">
+        <v>44209</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.45">

</xml_diff>